<commit_message>
Fixed a Parameter Name: TokenBoardAddress
</commit_message>
<xml_diff>
--- a/docs/jkbms send & receive frame data desc.xlsx
+++ b/docs/jkbms send & receive frame data desc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyMoore\Desktop\JK BMS ESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andy Docs\Andy Projects\PlatformIO\pwrGenie V2.0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E464FEB3-34D4-4D9E-AC0E-E53363F930DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA281AB6-7A6A-4371-92E5-9D46AF121C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37755" yWindow="2550" windowWidth="18225" windowHeight="23850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38100" yWindow="2895" windowWidth="18225" windowHeight="23850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="291">
   <si>
     <t>SOC</t>
   </si>
@@ -890,6 +890,9 @@
   </si>
   <si>
     <t>TokenLowCapacityAlarm</t>
+  </si>
+  <si>
+    <t>TokenBoardAddress</t>
   </si>
 </sst>
 </file>
@@ -989,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1044,26 +1047,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1397,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62790ACD-9666-FE45-B376-45B5FCF02634}">
-  <dimension ref="A1:EM88"/>
+  <dimension ref="A1:EM79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="DL16" sqref="DL16"/>
+    <sheetView tabSelected="1" topLeftCell="DC25" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="DL62" sqref="DL62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,12 +1699,12 @@
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.25">
       <c r="D4" s="8"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -1732,12 +1722,12 @@
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.25">
       <c r="D5" s="8"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -1821,7 +1811,7 @@
       <c r="W6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="X6" s="26"/>
+      <c r="X6" s="5"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3" t="s">
         <v>1</v>
@@ -1968,7 +1958,7 @@
       <c r="W7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="26"/>
+      <c r="X7" s="5"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3" t="s">
         <v>1</v>
@@ -2115,7 +2105,7 @@
       <c r="W8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="X8" s="26"/>
+      <c r="X8" s="5"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3" t="s">
         <v>1</v>
@@ -2262,7 +2252,7 @@
       <c r="W9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="X9" s="26"/>
+      <c r="X9" s="5"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3" t="s">
         <v>1</v>
@@ -2409,7 +2399,7 @@
       <c r="W10" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="X10" s="26"/>
+      <c r="X10" s="5"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3" t="s">
         <v>1</v>
@@ -2494,27 +2484,7 @@
       </c>
     </row>
     <row r="11" spans="1:115" x14ac:dyDescent="0.25">
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="31" t="s">
+      <c r="Y11" s="26" t="s">
         <v>266</v>
       </c>
       <c r="Z11" s="22">
@@ -2878,8 +2848,8 @@
       <c r="W12" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="32" t="s">
+      <c r="X12" s="5"/>
+      <c r="Y12" s="27" t="s">
         <v>262</v>
       </c>
       <c r="Z12" s="5" t="s">
@@ -3103,7 +3073,7 @@
       <c r="DJ12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="DK12" s="38"/>
+      <c r="DK12" s="29"/>
     </row>
     <row r="13" spans="1:115" x14ac:dyDescent="0.25">
       <c r="E13" s="18"/>
@@ -3123,11 +3093,10 @@
       <c r="U13" s="20"/>
       <c r="V13" s="20"/>
       <c r="W13" s="20"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="31" t="s">
+      <c r="Y13" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="AL13" s="24">
+      <c r="AL13">
         <f>HEX2DEC(AL12)</f>
         <v>60</v>
       </c>
@@ -3391,8 +3360,7 @@
       <c r="U14" s="20"/>
       <c r="V14" s="20"/>
       <c r="W14" s="20"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="31" t="s">
+      <c r="Y14" s="26" t="s">
         <v>264</v>
       </c>
       <c r="BC14">
@@ -3558,145 +3526,144 @@
       <c r="DK14" s="22"/>
     </row>
     <row r="15" spans="1:115" s="14" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="K15" s="42" t="s">
+      <c r="K15" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="L15" s="39" t="s">
+      <c r="L15" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="M15" s="43" t="s">
+      <c r="M15" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="N15" s="39" t="s">
+      <c r="N15" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="O15" s="44" t="s">
+      <c r="O15" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="P15" s="44" t="s">
+      <c r="P15" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="Q15" s="44" t="s">
+      <c r="Q15" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="R15" s="44" t="s">
+      <c r="R15" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="S15" s="40" t="s">
+      <c r="S15" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="T15" s="43" t="s">
+      <c r="T15" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="U15" s="43" t="s">
+      <c r="U15" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="V15" s="43" t="s">
+      <c r="V15" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="W15" s="43" t="s">
+      <c r="W15" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="33" t="s">
+      <c r="Y15" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="Z15" s="39" t="s">
+      <c r="Z15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="AA15" s="39" t="s">
+      <c r="AA15" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="AB15" s="40" t="s">
+      <c r="AB15" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="AC15" s="40" t="s">
+      <c r="AC15" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="AD15" s="41" t="s">
+      <c r="AD15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="AE15" s="41" t="s">
+      <c r="AE15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="AF15" s="41" t="s">
+      <c r="AF15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="AG15" s="41" t="s">
+      <c r="AG15" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="AH15" s="42" t="s">
+      <c r="AH15" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="AI15" s="39" t="s">
+      <c r="AI15" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="AJ15" s="43" t="s">
+      <c r="AJ15" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="AK15" s="39" t="s">
+      <c r="AK15" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="AL15" s="39" t="s">
+      <c r="AL15" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="BC15" s="39" t="s">
+      <c r="BC15" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="BD15" s="39" t="s">
+      <c r="BD15" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="BE15" s="39" t="s">
+      <c r="BE15" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="BF15" s="39" t="s">
+      <c r="BF15" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="BG15" s="39" t="s">
+      <c r="BG15" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="BH15" s="39" t="s">
+      <c r="BH15" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="BI15" s="39" t="s">
+      <c r="BI15" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="BJ15" s="39"/>
-      <c r="BK15" s="39"/>
-      <c r="BL15" s="39" t="s">
+      <c r="BJ15" s="30"/>
+      <c r="BK15" s="30"/>
+      <c r="BL15" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="DH15" s="39" t="s">
+      <c r="DH15" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="DI15" s="39" t="s">
+      <c r="DI15" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="DJ15" s="39" t="s">
+      <c r="DJ15" s="30" t="s">
         <v>97</v>
       </c>
       <c r="DK15" s="23"/>
@@ -3752,29 +3719,29 @@
       </c>
       <c r="DK16" s="23"/>
     </row>
-    <row r="17" spans="115:131" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="DK17" s="35" t="s">
+    <row r="17" spans="115:131" x14ac:dyDescent="0.25">
+      <c r="DK17" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="DL17" s="35" t="s">
+      <c r="DL17" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="DM17" s="35" t="s">
+      <c r="DM17" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="DN17" s="35"/>
-      <c r="DO17" s="35"/>
-      <c r="DP17" s="35"/>
-      <c r="DQ17" s="35"/>
-      <c r="DR17" s="35"/>
-      <c r="DS17" s="35"/>
-      <c r="DT17" s="35"/>
-      <c r="DU17" s="35"/>
-      <c r="DV17" s="35"/>
-      <c r="DW17" s="35" t="s">
+      <c r="DN17" s="18"/>
+      <c r="DO17" s="18"/>
+      <c r="DP17" s="18"/>
+      <c r="DQ17" s="18"/>
+      <c r="DR17" s="18"/>
+      <c r="DS17" s="18"/>
+      <c r="DT17" s="18"/>
+      <c r="DU17" s="18"/>
+      <c r="DV17" s="18"/>
+      <c r="DW17" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="DX17" s="35"/>
+      <c r="DX17" s="18"/>
     </row>
     <row r="18" spans="115:131" x14ac:dyDescent="0.25">
       <c r="DK18" s="22">
@@ -3792,7 +3759,7 @@
       <c r="DO18" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="DW18" s="24">
+      <c r="DW18">
         <f>HEX2DEC(RIGHT(DN18,2))*256+HEX2DEC(RIGHT(DO18,2))</f>
         <v>21</v>
       </c>
@@ -3814,7 +3781,7 @@
       <c r="DO19" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="DW19" s="24">
+      <c r="DW19">
         <f t="shared" ref="DW19:DW56" si="2">HEX2DEC(RIGHT(DN19,2))*256+HEX2DEC(RIGHT(DO19,2))</f>
         <v>16</v>
       </c>
@@ -3836,7 +3803,7 @@
       <c r="DO20" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="DW20" s="24">
+      <c r="DW20">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -3858,7 +3825,7 @@
       <c r="DO21" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="DW21" s="24">
+      <c r="DW21">
         <f t="shared" si="2"/>
         <v>7925</v>
       </c>
@@ -3891,7 +3858,7 @@
       <c r="DO22" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="DW22" s="24">
+      <c r="DW22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3910,11 +3877,11 @@
       <c r="DN23" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="DW23" s="24">
+      <c r="DW23">
         <f>HEX2DEC(RIGHT(DN23,2))</f>
         <v>87</v>
       </c>
-      <c r="DY23" s="25">
+      <c r="DY23" s="24">
         <f>DW23/100</f>
         <v>0.87</v>
       </c>
@@ -3933,7 +3900,7 @@
       <c r="DN24" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="DW24" s="24">
+      <c r="DW24">
         <f>HEX2DEC(RIGHT(DN24,2))</f>
         <v>2</v>
       </c>
@@ -3955,7 +3922,7 @@
       <c r="DO25" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="DW25" s="24">
+      <c r="DW25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3983,7 +3950,7 @@
       <c r="DQ26" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="DW26" s="24">
+      <c r="DW26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4005,7 +3972,7 @@
       <c r="DO27" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="DW27" s="24">
+      <c r="DW27">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -4031,7 +3998,7 @@
       <c r="DO28" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="DW28" s="24">
+      <c r="DW28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4053,7 +4020,7 @@
       <c r="DO29" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="DW29" s="24">
+      <c r="DW29">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -4078,7 +4045,7 @@
       <c r="DO30" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="DW30" s="24">
+      <c r="DW30">
         <f t="shared" si="2"/>
         <v>8400</v>
       </c>
@@ -4104,7 +4071,7 @@
       <c r="DO31" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="DW31" s="24">
+      <c r="DW31">
         <f t="shared" si="2"/>
         <v>5640</v>
       </c>
@@ -4130,7 +4097,7 @@
       <c r="DO32" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="DW32" s="24">
+      <c r="DW32">
         <f t="shared" si="2"/>
         <v>4200</v>
       </c>
@@ -4156,7 +4123,7 @@
       <c r="DO33" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="DW33" s="24">
+      <c r="DW33">
         <f t="shared" si="2"/>
         <v>4180</v>
       </c>
@@ -4182,7 +4149,7 @@
       <c r="DO34" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="DW34" s="24">
+      <c r="DW34">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -4204,7 +4171,7 @@
       <c r="DO35" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="DW35" s="24">
+      <c r="DW35">
         <f t="shared" si="2"/>
         <v>2820</v>
       </c>
@@ -4226,7 +4193,7 @@
       <c r="DO36" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="DW36" s="24">
+      <c r="DW36">
         <f t="shared" si="2"/>
         <v>2850</v>
       </c>
@@ -4248,7 +4215,7 @@
       <c r="DO37" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="DW37" s="24">
+      <c r="DW37">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -4270,7 +4237,7 @@
       <c r="DO38" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="DW38" s="24">
+      <c r="DW38">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
@@ -4295,7 +4262,7 @@
       <c r="DO39" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="DW39" s="24">
+      <c r="DW39">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -4317,7 +4284,7 @@
       <c r="DO40" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="DW40" s="24">
+      <c r="DW40">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
@@ -4339,7 +4306,7 @@
       <c r="DO41" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="DW41" s="24">
+      <c r="DW41">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -4361,7 +4328,7 @@
       <c r="DO42" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="DW42" s="24">
+      <c r="DW42">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
@@ -4383,7 +4350,7 @@
       <c r="DO43" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="DW43" s="24">
+      <c r="DW43">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
@@ -4408,7 +4375,7 @@
       <c r="DO44" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="DW44" s="24">
+      <c r="DW44">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -4430,7 +4397,7 @@
       <c r="DN45" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="DW45" s="24">
+      <c r="DW45">
         <f>HEX2DEC(RIGHT(DN45,2))</f>
         <v>1</v>
       </c>
@@ -4452,7 +4419,7 @@
       <c r="DO46" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="DW46" s="24">
+      <c r="DW46">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -4474,7 +4441,7 @@
       <c r="DO47" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="DW47" s="24">
+      <c r="DW47">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
@@ -4496,7 +4463,7 @@
       <c r="DO48" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="DW48" s="24">
+      <c r="DW48">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -4518,7 +4485,7 @@
       <c r="DO49" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="DW49" s="24">
+      <c r="DW49">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -4540,7 +4507,7 @@
       <c r="DO50" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="DW50" s="24">
+      <c r="DW50">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -4562,7 +4529,7 @@
       <c r="DO51" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="DW51" s="24">
+      <c r="DW51">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
@@ -4584,7 +4551,7 @@
       <c r="DO52" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="DW52" s="24">
+      <c r="DW52">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
@@ -4606,7 +4573,7 @@
       <c r="DO53" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="DW53" s="24">
+      <c r="DW53">
         <f t="shared" si="2"/>
         <v>65516</v>
       </c>
@@ -4628,7 +4595,7 @@
       <c r="DO54" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="DW54" s="24">
+      <c r="DW54">
         <f t="shared" si="2"/>
         <v>65526</v>
       </c>
@@ -4650,7 +4617,7 @@
       <c r="DO55" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="DW55" s="24">
+      <c r="DW55">
         <f t="shared" si="2"/>
         <v>65516</v>
       </c>
@@ -4672,7 +4639,7 @@
       <c r="DO56" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="DW56" s="24">
+      <c r="DW56">
         <f t="shared" si="2"/>
         <v>65526</v>
       </c>
@@ -4691,7 +4658,7 @@
       <c r="DN57" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="DW57" s="24">
+      <c r="DW57">
         <f>HEX2DEC(RIGHT(DN57,2))</f>
         <v>20</v>
       </c>
@@ -4734,7 +4701,7 @@
       <c r="DN59" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="DW59" s="24">
+      <c r="DW59">
         <f>HEX2DEC(RIGHT(DN59,2))</f>
         <v>1</v>
       </c>
@@ -4769,7 +4736,7 @@
         <v>203</v>
       </c>
       <c r="DL61" t="s">
-        <v>237</v>
+        <v>290</v>
       </c>
       <c r="DM61" s="8" t="s">
         <v>175</v>
@@ -4777,7 +4744,7 @@
       <c r="DN61" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="DW61" s="24">
+      <c r="DW61">
         <f>HEX2DEC(RIGHT(DN61,2))</f>
         <v>1</v>
       </c>
@@ -4796,7 +4763,7 @@
       <c r="DN62" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="DW62" s="24">
+      <c r="DW62">
         <f>HEX2DEC(RIGHT(DN62,2))</f>
         <v>1</v>
       </c>
@@ -4833,7 +4800,7 @@
       <c r="DN64" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="DW64" s="24">
+      <c r="DW64">
         <f>HEX2DEC(RIGHT(DN64,2))</f>
         <v>20</v>
       </c>
@@ -4894,7 +4861,7 @@
       <c r="DN66" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="DW66" s="24">
+      <c r="DW66">
         <f>HEX2DEC(RIGHT(DN66,2))</f>
         <v>0</v>
       </c>
@@ -5054,7 +5021,7 @@
       <c r="DN71" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="DW71" s="24">
+      <c r="DW71">
         <f>HEX2DEC(RIGHT(DN71,2))</f>
         <v>0</v>
       </c>
@@ -5215,7 +5182,7 @@
         <f>DK76+4</f>
         <v>298</v>
       </c>
-      <c r="DL77" s="35" t="s">
+      <c r="DL77" s="18" t="s">
         <v>261</v>
       </c>
       <c r="DM77" s="8" t="s">
@@ -5227,7 +5194,7 @@
         <f>DK77+1</f>
         <v>299</v>
       </c>
-      <c r="DL78" s="36" t="s">
+      <c r="DL78" s="20" t="s">
         <v>260</v>
       </c>
       <c r="DM78" s="8" t="s">
@@ -5244,91 +5211,13 @@
       </c>
     </row>
     <row r="79" spans="115:143" x14ac:dyDescent="0.25">
-      <c r="DK79" s="31">
+      <c r="DK79" s="26">
         <f>DK78+4</f>
         <v>303</v>
       </c>
-      <c r="DL79" s="30" t="s">
+      <c r="DL79" s="25" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="83" spans="116:126" x14ac:dyDescent="0.25">
-      <c r="DL83" s="27"/>
-      <c r="DM83" s="27"/>
-      <c r="DN83" s="27"/>
-      <c r="DO83" s="27"/>
-      <c r="DP83" s="27"/>
-      <c r="DQ83" s="27"/>
-      <c r="DR83" s="27"/>
-      <c r="DS83" s="27"/>
-      <c r="DT83" s="27"/>
-      <c r="DU83" s="27"/>
-      <c r="DV83" s="27"/>
-    </row>
-    <row r="84" spans="116:126" x14ac:dyDescent="0.25">
-      <c r="DL84" s="27"/>
-      <c r="DM84" s="27"/>
-      <c r="DN84" s="27"/>
-      <c r="DO84" s="27"/>
-      <c r="DP84" s="27"/>
-      <c r="DQ84" s="27"/>
-      <c r="DR84" s="27"/>
-      <c r="DS84" s="27"/>
-      <c r="DT84" s="27"/>
-      <c r="DU84" s="27"/>
-      <c r="DV84" s="27"/>
-    </row>
-    <row r="85" spans="116:126" x14ac:dyDescent="0.25">
-      <c r="DL85" s="27"/>
-      <c r="DM85" s="37"/>
-      <c r="DN85" s="37"/>
-      <c r="DO85" s="37"/>
-      <c r="DP85" s="27"/>
-      <c r="DQ85" s="27"/>
-      <c r="DR85" s="37"/>
-      <c r="DS85" s="37"/>
-      <c r="DT85" s="37"/>
-      <c r="DU85" s="27"/>
-      <c r="DV85" s="27"/>
-    </row>
-    <row r="86" spans="116:126" x14ac:dyDescent="0.25">
-      <c r="DL86" s="27"/>
-      <c r="DM86" s="27"/>
-      <c r="DN86" s="27"/>
-      <c r="DO86" s="27"/>
-      <c r="DP86" s="27"/>
-      <c r="DQ86" s="27"/>
-      <c r="DR86" s="27"/>
-      <c r="DS86" s="27"/>
-      <c r="DT86" s="27"/>
-      <c r="DU86" s="27"/>
-      <c r="DV86" s="27"/>
-    </row>
-    <row r="87" spans="116:126" x14ac:dyDescent="0.25">
-      <c r="DL87" s="27"/>
-      <c r="DM87" s="27"/>
-      <c r="DN87" s="27"/>
-      <c r="DO87" s="27"/>
-      <c r="DP87" s="27"/>
-      <c r="DQ87" s="27"/>
-      <c r="DR87" s="27"/>
-      <c r="DS87" s="27"/>
-      <c r="DT87" s="27"/>
-      <c r="DU87" s="27"/>
-      <c r="DV87" s="27"/>
-    </row>
-    <row r="88" spans="116:126" x14ac:dyDescent="0.25">
-      <c r="DL88" s="27"/>
-      <c r="DM88" s="27"/>
-      <c r="DN88" s="27"/>
-      <c r="DO88" s="27"/>
-      <c r="DP88" s="27"/>
-      <c r="DQ88" s="27"/>
-      <c r="DR88" s="27"/>
-      <c r="DS88" s="27"/>
-      <c r="DT88" s="27"/>
-      <c r="DU88" s="27"/>
-      <c r="DV88" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>